<commit_message>
Partial implementation of rich text for dialogue
Dialogue can now be written in Unity's rich text format. Bugs occur if tags are nested, however (to be fixed).
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -53,12 +53,6 @@
     <t>frog_mario</t>
   </si>
   <si>
-    <t>Hey you! You're walking in the wrong part of town.</t>
-  </si>
-  <si>
-    <t>Ribbit Ribbit! (Yeah frog-face! Wrong part of town!)</t>
-  </si>
-  <si>
     <t>Let's get em!</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>1, 1</t>
+  </si>
+  <si>
+    <t>Ribbit &lt;i&gt;Ribbit!&lt;/i&gt; (Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)</t>
+  </si>
+  <si>
+    <t>&lt;size=48&gt;Hey you!&lt;/size&gt; You're walking in the &lt;color=red&gt;wrong&lt;/color&gt; part of town.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -464,19 +464,19 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -487,19 +487,19 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -510,25 +510,25 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Finished basic rich text implementation
Text dialogue fully supports Unity's built in rich text tags. We have NOT yet added support for custom tags with custom effects.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -77,10 +77,10 @@
     <t>1, 1</t>
   </si>
   <si>
-    <t>Ribbit &lt;i&gt;Ribbit!&lt;/i&gt; (Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)</t>
-  </si>
-  <si>
     <t>&lt;size=48&gt;Hey you!&lt;/size&gt; You're walking in the &lt;color=red&gt;wrong&lt;/color&gt; part of town.</t>
+  </si>
+  <si>
+    <t>Ribbit &lt;i&gt;Ribbit!&lt;/i&gt; &lt;size=24&gt;(Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)&lt;/size&gt;</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +464,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fixed the Mergepocalypse bugs
-I had unity rebuild all of the assets, then mostly just restarted the project a bunch until it figured itself out. Then I just hooked everything out, reformatted the excels, and added some functionality back in
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -439,6 +439,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1">

</xml_diff>

<commit_message>
Added relational spreadsheet capabilities, fixed tag bug
You can now specify a link to another gameflow file within the main gameflow file for simplicity and modularity by using the LINK tag.

Links can be infinitely nested, but loops will cause an infinite loop.

Also, fixed a bug where tags wouldn't be cleared after a line of dialogue.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>DIALOGUE</t>
-  </si>
-  <si>
-    <t>END_GAME</t>
   </si>
   <si>
     <t>Tanuki</t>
@@ -432,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,19 +445,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -480,10 +495,10 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -491,61 +506,33 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TextEvents for effects that occur during dialogue
TextEvents.cs contains all the functions that can be run during text dialogue (currently, only a momentary screen shake). To add a new event, make a function that matches the TextEventDel delegate, put it in the class, and then add the function to the text_event_map Dictionary.

Events are specified in the gameflow dialogue files with square brackets. Format is [event-name=option1,option2,...]
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -50,9 +50,6 @@
     <t>frog_mario</t>
   </si>
   <si>
-    <t>Let's get em!</t>
-  </si>
-  <si>
     <t>jazzy_retro_battle_theme</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Ribbit &lt;i&gt;Ribbit!&lt;/i&gt; &lt;size=24&gt;(Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>Let's [screen-shake=0.2,0.3]get em!</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -463,19 +463,19 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -486,19 +486,19 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -509,25 +509,25 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added floating text effect
Text can be displayed at the center of the screen during dialogue.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -89,10 +89,10 @@
     <t>[block=t]Rib[pause=1]bit[pause=1][block=f] &lt;i&gt;Ribbit!&lt;/i&gt; &lt;size=24&gt;(Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)&lt;/size&gt;</t>
   </si>
   <si>
-    <t>[block=t][fade=out,2]Wait, why is the screen fading away?[pause=6][next]</t>
-  </si>
-  <si>
-    <t>[fade=in,0][screen-shake=0.2,0.5]BOO![block=f]</t>
+    <t>[fade=in,0,0,0,0][screen-shake=0.2,0.5]BOO![block=f]</t>
+  </si>
+  <si>
+    <t>[block=t][fade=out,2,0,0,0]Wait, why is the screen fading away?[pause=2][center-text-fade=in,0][center-text-scroll=0.05,0,0,0,SPOOPY][pause=2][center-text-fade=out,2][pause=3][next]</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -576,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added more text events
Added hiding/showing the text box.
Added changing the talking sfx.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -71,28 +71,16 @@
     <t>1, 1</t>
   </si>
   <si>
-    <t>Let's [screen-shake=0.2,0.3]get em!</t>
-  </si>
-  <si>
-    <t>[block=t]&lt;size=48&gt;Hey you!&lt;/size&gt;[block=f] You're walking in the &lt;color=red&gt;wrong&lt;/color&gt; part of town.</t>
-  </si>
-  <si>
-    <t>CENTER</t>
-  </si>
-  <si>
-    <t>STOP</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>[block=t]Rib[pause=1]bit[pause=1][block=f] &lt;i&gt;Ribbit!&lt;/i&gt; &lt;size=24&gt;(Yeah &lt;color=green&gt;frog-face!&lt;/color&gt; Wrong part of town!)&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>[fade=in,0,0,0,0][screen-shake=0.2,0.5]BOO![block=f]</t>
-  </si>
-  <si>
-    <t>[block=t][fade=out,2,0,0,0][play-sfx=OTHER,Static_Sound]Wait, why is the screen fading away?[pause=2][center-text-fade=in,0][center-text-scroll=0.05,0,0,0,SPOOPY][pause=2][center-text-fade=out,2][pause=3][next]</t>
+    <t>Hmmmmm</t>
+  </si>
+  <si>
+    <t>[set-talk-sfx=take_damage]Hmm</t>
+  </si>
+  <si>
+    <t>END_GAME</t>
+  </si>
+  <si>
+    <t>Im going to disappear[hide-text-box=t][set-talk-sfx=_] And then will you see me now?[hide-text-box=f]</t>
   </si>
 </sst>
 </file>
@@ -447,7 +435,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,37 +448,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
+      <c r="A1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -498,19 +468,19 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -521,27 +491,21 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -550,50 +514,38 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented basic in dialogue input prompting
Dialogue can now prompt input from player (like for the player's name).

Player information is stored in a static instance of 'PlayerDialogueInfo'.

Currently, only 'name' input is supported (and is, in fact, the default).
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Tanuki</t>
   </si>
   <si>
-    <t>Frog</t>
-  </si>
-  <si>
     <t>tanuki_mario</t>
   </si>
   <si>
@@ -53,12 +50,6 @@
     <t>jazzy_retro_battle_theme</t>
   </si>
   <si>
-    <t>frogs</t>
-  </si>
-  <si>
-    <t>LEFT</t>
-  </si>
-  <si>
     <t>RIGHT</t>
   </si>
   <si>
@@ -71,16 +62,19 @@
     <t>1, 1</t>
   </si>
   <si>
-    <t>Hmmmmm</t>
-  </si>
-  <si>
-    <t>[set-talk-sfx=take_damage]Hmm</t>
-  </si>
-  <si>
     <t>END_GAME</t>
   </si>
   <si>
-    <t>Im going to disappear[hide-text-box=t][set-talk-sfx=_] And then will you see me now?[hide-text-box=f]</t>
+    <t>enter your name.</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>[prompt=name].</t>
+  </si>
+  <si>
+    <t>good name.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +429,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -471,42 +465,33 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -517,25 +502,25 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -545,7 +530,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dialogue macro substitution system
Things specified with {} in dialogue are replaced with appropriate strings (like the player's name).

Currently, only the name is implemented.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/cutscene_tests.xlsx
+++ b/Typocrypha/Assets/excel/cutscene_tests.xlsx
@@ -74,7 +74,7 @@
     <t>[prompt=name].</t>
   </si>
   <si>
-    <t>good name.</t>
+    <t>{name}? good name.</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>